<commit_message>
Error in Ambient Heat Gas Heat Pump
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_RSD_NewTechs_Trans.xlsx
+++ b/SubRES_TMPL/SubRES_RSD_NewTechs_Trans.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{365E8C69-DD82-4ED3-979D-0706F3AD5598}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209BB8C2-5FB4-475F-B1F3-D281EBB926D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="819" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15006,8 +15006,8 @@
   </sheetPr>
   <dimension ref="A1:H89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F85" sqref="F85"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -15218,8 +15218,8 @@
         <v>182</v>
       </c>
       <c r="F12" s="32" t="str">
-        <f>"R-S*_"&amp;A12&amp;"_"&amp;B12&amp;",-*HPN*"</f>
-        <v>R-S*_Apt_GAS,-*HPN*</v>
+        <f>"R-S*_"&amp;A12&amp;"_"&amp;B12&amp;"*"</f>
+        <v>R-S*_Apt_GAS*</v>
       </c>
       <c r="G12" s="32" t="str">
         <f>IFERROR("*"&amp;AVERAGEIFS('BY-RSD-EFF'!$L$2:$L$100,'BY-RSD-EFF'!$C$2:$C$100,EFF!C12,'BY-RSD-EFF'!$A$2:$A$100,"BASE"),"")</f>
@@ -15503,8 +15503,8 @@
         <v>182</v>
       </c>
       <c r="F25" s="32" t="str">
-        <f>"R-S*_"&amp;A25&amp;"_"&amp;B25&amp;",-*HPN*"</f>
-        <v>R-S*_Att_GAS,-*HPN*</v>
+        <f>"R-S*_"&amp;A25&amp;"_"&amp;B25&amp;"*"</f>
+        <v>R-S*_Att_GAS*</v>
       </c>
       <c r="G25" s="32" t="str">
         <f>IFERROR("*"&amp;AVERAGEIFS('BY-RSD-EFF'!$L$2:$L$100,'BY-RSD-EFF'!$C$2:$C$100,EFF!C25,'BY-RSD-EFF'!$A$2:$A$100,"BASE"),"")</f>
@@ -15791,8 +15791,8 @@
         <v>182</v>
       </c>
       <c r="F38" s="32" t="str">
-        <f>"R-S*_"&amp;A38&amp;"_"&amp;B38&amp;",-*HPN*"</f>
-        <v>R-S*_Det_GAS,-*HPN*</v>
+        <f>"R-S*_"&amp;A38&amp;"_"&amp;B38&amp;"*"</f>
+        <v>R-S*_Det_GAS*</v>
       </c>
       <c r="G38" s="32" t="str">
         <f>IFERROR("*"&amp;AVERAGEIFS('BY-RSD-EFF'!$L$2:$L$100,'BY-RSD-EFF'!$C$2:$C$100,EFF!C38,'BY-RSD-EFF'!$A$2:$A$100,"BASE"),"")</f>

</xml_diff>

<commit_message>
Prepare new/modified files for a release
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_RSD_NewTechs_Trans.xlsx
+++ b/SubRES_TMPL/SubRES_RSD_NewTechs_Trans.xlsx
@@ -2,15 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SubRES_TMPL\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB46D3D7-A6EE-48B8-8D99-4EDECE320029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{624B4313-94CA-478D-80F8-5CCE4176A4FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" tabRatio="819" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" tabRatio="819" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="65" r:id="rId1"/>
@@ -32,9 +27,6 @@
     <sheet name="BY-RSD-RF" sheetId="50" r:id="rId17"/>
     <sheet name="BY-RSD-OE" sheetId="59" r:id="rId18"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId19"/>
-  </externalReferences>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="__123Graph_AEUMILKPN" hidden="1">#REF!</definedName>
@@ -74,7 +66,6 @@
     <definedName name="elecc" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elecc" localSheetId="2" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elecc" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
-    <definedName name="FID_1">[1]AGR_Fuels!$A$2</definedName>
     <definedName name="IQ_FWD_CY" hidden="1">10001</definedName>
     <definedName name="IQ_FWD_CY1" hidden="1">10002</definedName>
     <definedName name="IQ_FWD_CY2" hidden="1">10003</definedName>
@@ -135,7 +126,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>Alessandro Chiodi</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="D123" authorId="0" shapeId="0" xr:uid="{252C524F-867C-494B-8549-0779FBA2A96C}">
@@ -148,7 +139,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Alessandro Chiodi:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -172,7 +163,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Alessandro Chiodi:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -196,7 +187,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Alessandro Chiodi:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -220,7 +211,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Alessandro Chiodi:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -244,7 +235,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Alessandro Chiodi:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -268,7 +259,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Alessandro Chiodi:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -292,7 +283,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Alessandro Chiodi:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -313,7 +304,7 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>Alessandro Chiodi</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="E15" authorId="0" shapeId="0" xr:uid="{5E2488D4-DAF1-46AB-A539-E1B33B9CF9CE}">
@@ -395,7 +386,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Alessandro Chiodi:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -419,7 +410,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Alessandro Chiodi:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -443,7 +434,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Alessandro Chiodi:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -467,7 +458,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Alessandro Chiodi:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -492,7 +483,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Alessandro Chiodi:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -517,7 +508,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Alessandro Chiodi:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -559,7 +550,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2707" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2708" uniqueCount="296">
   <si>
     <t>IE</t>
   </si>
@@ -1462,6 +1453,9 @@
   </si>
   <si>
     <t>New Technologies - Transformation</t>
+  </si>
+  <si>
+    <t>1.0.0-s.1</t>
   </si>
 </sst>
 </file>
@@ -2060,7 +2054,7 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect l="4620" t="8935" r="7748" b="12927"/>
+        <a:srcRect/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -2261,7 +2255,7 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect l="4000" t="26200" r="4000" b="26199"/>
+        <a:srcRect/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
@@ -2350,141 +2344,6 @@
     <mc:Fallback/>
   </mc:AlternateContent>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="IEA Data"/>
-      <sheetName val="E&amp;D Drivers"/>
-      <sheetName val="AGR_Fuels"/>
-      <sheetName val="AGR"/>
-      <sheetName val="RES_Fuels"/>
-      <sheetName val="RH1"/>
-      <sheetName val="RH2"/>
-      <sheetName val="RH3"/>
-      <sheetName val="RH4"/>
-      <sheetName val="RC1"/>
-      <sheetName val="RC2"/>
-      <sheetName val="RC3"/>
-      <sheetName val="RC4"/>
-      <sheetName val="RHW"/>
-      <sheetName val="RRF"/>
-      <sheetName val="RCW"/>
-      <sheetName val="RCD"/>
-      <sheetName val="RK1"/>
-      <sheetName val="RK2"/>
-      <sheetName val="RK3"/>
-      <sheetName val="RK4"/>
-      <sheetName val="RDW"/>
-      <sheetName val="RME"/>
-      <sheetName val="RL1"/>
-      <sheetName val="RL2"/>
-      <sheetName val="RL3"/>
-      <sheetName val="RL4"/>
-      <sheetName val="COM_Fuels"/>
-      <sheetName val="CH1"/>
-      <sheetName val="CH2"/>
-      <sheetName val="CH3"/>
-      <sheetName val="CH4"/>
-      <sheetName val="CC1"/>
-      <sheetName val="CC2"/>
-      <sheetName val="CC3"/>
-      <sheetName val="CC4"/>
-      <sheetName val="CHW"/>
-      <sheetName val="CAA"/>
-      <sheetName val="CLA"/>
-      <sheetName val="ElastPar"/>
-      <sheetName val="Conversion Factors"/>
-      <sheetName val="Intro"/>
-      <sheetName val="TechRep"/>
-      <sheetName val="Other_HYDRO"/>
-      <sheetName val="Other_NUCL"/>
-      <sheetName val="Other_THERM"/>
-      <sheetName val="Other_CHP"/>
-      <sheetName val="Other_RENEW"/>
-      <sheetName val="Other_HEAT"/>
-      <sheetName val="ELC_FUELS"/>
-      <sheetName val="ELC"/>
-      <sheetName val="HEAT"/>
-      <sheetName val="CHP"/>
-      <sheetName val="ELC_EMI"/>
-      <sheetName val="Constant Table"/>
-      <sheetName val="ANS_ITEMS_DEL"/>
-      <sheetName val="ANS_ITEMS"/>
-      <sheetName val="ANS_TIDDATA"/>
-      <sheetName val="ANS_TSDATA"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1">
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>^FI_ST: TCH, PRC</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
-      <sheetData sheetId="27" refreshError="1"/>
-      <sheetData sheetId="28" refreshError="1"/>
-      <sheetData sheetId="29" refreshError="1"/>
-      <sheetData sheetId="30" refreshError="1"/>
-      <sheetData sheetId="31" refreshError="1"/>
-      <sheetData sheetId="32" refreshError="1"/>
-      <sheetData sheetId="33" refreshError="1"/>
-      <sheetData sheetId="34" refreshError="1"/>
-      <sheetData sheetId="35" refreshError="1"/>
-      <sheetData sheetId="36" refreshError="1"/>
-      <sheetData sheetId="37" refreshError="1"/>
-      <sheetData sheetId="38" refreshError="1"/>
-      <sheetData sheetId="39" refreshError="1"/>
-      <sheetData sheetId="40" refreshError="1"/>
-      <sheetData sheetId="41" refreshError="1"/>
-      <sheetData sheetId="42" refreshError="1"/>
-      <sheetData sheetId="43" refreshError="1"/>
-      <sheetData sheetId="44" refreshError="1"/>
-      <sheetData sheetId="45" refreshError="1"/>
-      <sheetData sheetId="46" refreshError="1"/>
-      <sheetData sheetId="47" refreshError="1"/>
-      <sheetData sheetId="48" refreshError="1"/>
-      <sheetData sheetId="49" refreshError="1"/>
-      <sheetData sheetId="50" refreshError="1"/>
-      <sheetData sheetId="51" refreshError="1"/>
-      <sheetData sheetId="52" refreshError="1"/>
-      <sheetData sheetId="53" refreshError="1"/>
-      <sheetData sheetId="54" refreshError="1"/>
-      <sheetData sheetId="55" refreshError="1"/>
-      <sheetData sheetId="56" refreshError="1"/>
-      <sheetData sheetId="57" refreshError="1"/>
-      <sheetData sheetId="58" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2811,7 +2670,9 @@
   <sheetPr codeName="Sheet18"/>
   <dimension ref="A1:Z99"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30:D30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -3643,8 +3504,8 @@
       <c r="A29" s="49" t="s">
         <v>283</v>
       </c>
-      <c r="B29" s="53">
-        <v>1</v>
+      <c r="B29" s="53" t="s">
+        <v>295</v>
       </c>
       <c r="C29" s="52"/>
       <c r="D29" s="52"/>
@@ -8794,6 +8655,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -8890,6 +8752,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -9068,6 +8931,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -9164,6 +9028,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -9347,6 +9212,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -9443,6 +9309,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -9623,6 +9490,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -9721,6 +9589,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -9819,6 +9688,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -10855,6 +10725,7 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
@@ -11719,7 +11590,7 @@
   </sheetPr>
   <dimension ref="A1:L135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
@@ -15035,7 +14906,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -16964,7 +16836,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -18624,6 +18497,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -20158,5 +20032,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Error in LST something to do with R-SH_Det_ELC_XO
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_RSD_NewTechs_Trans.xlsx
+++ b/SubRES_TMPL/SubRES_RSD_NewTechs_Trans.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A959307-0502-4A74-887A-90EA90FA5D00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FCEBEEC-0EAF-4211-9AD5-0F5AC502020F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="819" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="819" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="65" r:id="rId1"/>
@@ -34,7 +34,6 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId19"/>
-    <externalReference r:id="rId20"/>
   </externalReferences>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" localSheetId="0" hidden="1">#REF!</definedName>
@@ -2525,29 +2524,6 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Cover"/>
-      <sheetName val="Regions"/>
-      <sheetName val="TechSelection"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="3">
-          <cell r="C3" t="str">
-            <v>IE</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -10743,8 +10719,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B3:AH7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4:AH5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10815,7 +10791,7 @@
         <v>8</v>
       </c>
       <c r="H4" s="5" t="str">
-        <f>[2]Regions!C3</f>
+        <f>Regions!C3</f>
         <v>IE</v>
       </c>
       <c r="I4" s="6" t="s">
@@ -11897,8 +11873,8 @@
   </sheetPr>
   <dimension ref="A1:L141"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12543,8 +12519,8 @@
         <v>83</v>
       </c>
       <c r="H23" s="31" t="str">
-        <f>"R-SH*"&amp;F23&amp;"_"&amp;G23&amp;"*X1"</f>
-        <v>R-SH*Att_ELC*X1</v>
+        <f>"R-SH_"&amp;F23&amp;"_"&amp;G23&amp;"_X1"</f>
+        <v>R-SH_Att_ELC_X1</v>
       </c>
       <c r="J23" s="32" t="s">
         <v>78</v>
@@ -12577,8 +12553,8 @@
         <v>83</v>
       </c>
       <c r="H24" s="32" t="str">
-        <f>"R-SH*"&amp;F23&amp;"_"&amp;G23&amp;"*X0"</f>
-        <v>R-SH*Att_ELC*X0</v>
+        <f>"R-SH_"&amp;F23&amp;"_"&amp;G23&amp;"_X0"</f>
+        <v>R-SH_Att_ELC_X0</v>
       </c>
       <c r="J24" s="32"/>
       <c r="K24" s="32"/>

</xml_diff>

<commit_message>
Error in RSD Trans file -
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_RSD_NewTechs_Trans.xlsx
+++ b/SubRES_TMPL/SubRES_RSD_NewTechs_Trans.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FCEBEEC-0EAF-4211-9AD5-0F5AC502020F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E5D3BD3-B114-4D56-8570-A7630AE15376}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="819" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11873,8 +11873,8 @@
   </sheetPr>
   <dimension ref="A1:L141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12139,8 +12139,8 @@
         <v>244</v>
       </c>
       <c r="B11" s="32" t="str">
-        <f>"R-S*_"&amp;F11&amp;"_"&amp;G11&amp;"_N1"&amp;",-R-SC*"</f>
-        <v>R-S*_Apt_ELC_N1,-R-SC*</v>
+        <f>"R-S*_"&amp;F11&amp;"_"&amp;G11&amp;"_N1"</f>
+        <v>R-S*_Apt_ELC_N1</v>
       </c>
       <c r="C11" s="32"/>
       <c r="D11" s="56">
@@ -12538,8 +12538,8 @@
         <v>244</v>
       </c>
       <c r="B24" s="32" t="str">
-        <f>"R-S*_"&amp;F24&amp;"_"&amp;G24&amp;"_N1"&amp;",-R-SC*"</f>
-        <v>R-S*_Att_ELC_N1,-R-SC*</v>
+        <f>"R-S*_"&amp;F24&amp;"_"&amp;G24&amp;"_N1"&amp;""</f>
+        <v>R-S*_Att_ELC_N1</v>
       </c>
       <c r="C24" s="32"/>
       <c r="D24" s="56">
@@ -12874,8 +12874,8 @@
         <v>244</v>
       </c>
       <c r="B39" s="32" t="str">
-        <f>"R-S*_"&amp;F39&amp;"_"&amp;G39&amp;"_N1"&amp;",-R-SC*"</f>
-        <v>R-S*_Det_ELC_N1,-R-SC*</v>
+        <f>"R-S*_"&amp;F39&amp;"_"&amp;G39&amp;"_N1"</f>
+        <v>R-S*_Det_ELC_N1</v>
       </c>
       <c r="C39" s="32"/>
       <c r="D39" s="56">
@@ -13215,8 +13215,8 @@
         <v>198</v>
       </c>
       <c r="B54" s="32" t="str">
-        <f>"R-S*_"&amp;F54&amp;"_"&amp;G54&amp;"_N1"&amp;",-R-SC*"</f>
-        <v>R-S*_Apt_ELC_N1,-R-SC*</v>
+        <f>"R-S*_"&amp;F54&amp;"_"&amp;G54&amp;"_N1"</f>
+        <v>R-S*_Apt_ELC_N1</v>
       </c>
       <c r="C54" s="32" t="s">
         <v>296</v>
@@ -13539,8 +13539,8 @@
         <v>198</v>
       </c>
       <c r="B67" s="32" t="str">
-        <f>"R-S*_"&amp;F67&amp;"_"&amp;G67&amp;"_N1"&amp;",-R-SC*"</f>
-        <v>R-S*_Att_ELC_N1,-R-SC*</v>
+        <f>"R-S*_"&amp;F67&amp;"_"&amp;G67&amp;"_N1"</f>
+        <v>R-S*_Att_ELC_N1</v>
       </c>
       <c r="C67" s="32" t="s">
         <v>298</v>
@@ -13899,8 +13899,8 @@
         <v>198</v>
       </c>
       <c r="B82" s="32" t="str">
-        <f>"R-S*_"&amp;F82&amp;"_"&amp;G82&amp;"_N1"&amp;",-R-SC*"</f>
-        <v>R-S*_Det_ELC_N1,-R-SC*</v>
+        <f>"R-S*_"&amp;F82&amp;"_"&amp;G82&amp;"_N1"</f>
+        <v>R-S*_Det_ELC_N1</v>
       </c>
       <c r="C82" s="32"/>
       <c r="D82" s="56">

</xml_diff>

<commit_message>
Update availability factors for private cars in the ILED scenario
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_RSD_NewTechs_Trans.xlsx
+++ b/SubRES_TMPL/SubRES_RSD_NewTechs_Trans.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIM-2.0\times-ireland-model-ILED\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAF60D87-E273-42CE-AB0A-4F4370453A65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3131966B-E8E1-45C8-9F02-CC7919EC9D96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="760" windowWidth="14400" windowHeight="7360" tabRatio="819" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25260" yWindow="2772" windowWidth="14400" windowHeight="7356" tabRatio="819" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="65" r:id="rId1"/>

</xml_diff>

<commit_message>
Address domain violation error
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_RSD_NewTechs_Trans.xlsx
+++ b/SubRES_TMPL/SubRES_RSD_NewTechs_Trans.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4121C59A-C3BC-4714-9E31-31608A84AC3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0308F661-8C72-417A-8165-567B850378B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="105" yWindow="345" windowWidth="21600" windowHeight="11295" tabRatio="819" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="819" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="65" r:id="rId1"/>
@@ -559,7 +559,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2773" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2774" uniqueCount="302">
   <si>
     <t>IE</t>
   </si>
@@ -11736,9 +11736,7 @@
   </sheetPr>
   <dimension ref="A1:L141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -13786,7 +13784,9 @@
         <f>"R-S*_"&amp;F82&amp;"_"&amp;G82&amp;"_N1"&amp;",-R-SC*"</f>
         <v>R-S*_Det_ELC_N1,-R-SC*</v>
       </c>
-      <c r="C82" s="31"/>
+      <c r="C82" s="31" t="s">
+        <v>300</v>
+      </c>
       <c r="D82" s="54">
         <f t="shared" si="17"/>
         <v>4.5630448521753401E-2</v>

</xml_diff>

<commit_message>
HVO trans file update
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_RSD_NewTechs_Trans.xlsx
+++ b/SubRES_TMPL/SubRES_RSD_NewTechs_Trans.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B8744C-59FF-4A24-A4DC-55C956E0DD4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACFC9ABB-E3D3-4203-A167-AC0EDD5F5E39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="819" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="819" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="65" r:id="rId1"/>
@@ -1398,18 +1398,6 @@
     <t>R-SW_Det_FPL*</t>
   </si>
   <si>
-    <t>R-SH_Att_HVO*</t>
-  </si>
-  <si>
-    <t>R-SH_Det_HVO*</t>
-  </si>
-  <si>
-    <t>R-SW_Att_HVO*</t>
-  </si>
-  <si>
-    <t>R-SW_Det_HVO*</t>
-  </si>
-  <si>
     <t>TIMES-Ireland Model</t>
   </si>
   <si>
@@ -1492,6 +1480,18 @@
   </si>
   <si>
     <t>Added Regions</t>
+  </si>
+  <si>
+    <t>R-SH_Att_BDL*</t>
+  </si>
+  <si>
+    <t>R-SH_Det_BDL*</t>
+  </si>
+  <si>
+    <t>R-SW_Att_BDL*</t>
+  </si>
+  <si>
+    <t>R-SW_Det_BDL*</t>
   </si>
 </sst>
 </file>
@@ -3270,7 +3270,7 @@
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="58" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B16" s="58"/>
       <c r="C16" s="58"/>
@@ -3356,10 +3356,10 @@
     </row>
     <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="43" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B19" s="57" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="C19" s="57"/>
       <c r="D19" s="57"/>
@@ -3388,10 +3388,10 @@
     </row>
     <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="43" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="B20" s="57" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="C20" s="57"/>
       <c r="D20" s="57"/>
@@ -3420,10 +3420,10 @@
     </row>
     <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="43" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B21" s="46" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C21" s="46"/>
       <c r="D21" s="46"/>
@@ -3480,10 +3480,10 @@
     </row>
     <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="43" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B23" s="57" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="C23" s="57"/>
       <c r="D23" s="57"/>
@@ -3513,7 +3513,7 @@
     <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="43"/>
       <c r="B24" s="57" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C24" s="57"/>
       <c r="D24" s="57"/>
@@ -3543,7 +3543,7 @@
     <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="43"/>
       <c r="B25" s="57" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="C25" s="57"/>
       <c r="D25" s="57"/>
@@ -3572,10 +3572,10 @@
     </row>
     <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="43" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="B26" s="57" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="C26" s="57"/>
       <c r="D26" s="57"/>
@@ -3605,7 +3605,7 @@
     <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="43"/>
       <c r="B27" s="57" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="C27" s="57"/>
       <c r="D27" s="57"/>
@@ -3662,7 +3662,7 @@
     </row>
     <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="43" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B29" s="47">
         <v>1</v>
@@ -3694,10 +3694,10 @@
     </row>
     <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="43" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B30" s="59" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C30" s="57"/>
       <c r="D30" s="57"/>
@@ -3726,10 +3726,10 @@
     </row>
     <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="43" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B31" s="57" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="C31" s="57"/>
       <c r="D31" s="57"/>
@@ -3759,7 +3759,7 @@
     <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="49"/>
       <c r="B32" s="50" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C32" s="49"/>
       <c r="D32" s="49"/>
@@ -15004,13 +15004,13 @@
         <v>44726</v>
       </c>
       <c r="B6" s="55" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="C6" s="55" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="E6" s="55" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -15025,7 +15025,7 @@
   <dimension ref="A3:AD37"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -15790,7 +15790,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B3:AA7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
@@ -16810,8 +16810,8 @@
   </sheetPr>
   <dimension ref="A1:L141"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -16905,7 +16905,7 @@
         <v>R-SH*Apt_COA*</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D6" s="51">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,B6,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
@@ -16942,7 +16942,7 @@
         <v>R-SH*Apt_BDL*</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D7" s="52">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,B7,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
@@ -16979,7 +16979,7 @@
         <v>R-SH*Apt_ETH*</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D8" s="51">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,B8,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
@@ -17016,7 +17016,7 @@
         <v>R-SH*Apt_LPG*</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D9" s="52">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,B9,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
@@ -17053,7 +17053,7 @@
         <v>R-S*_Apt*HPN*</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D10" s="51">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H10,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
@@ -17090,7 +17090,7 @@
         <v>R-S*_Apt_ELC_N1,-R-SC*</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D11" s="52">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H11,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
@@ -17127,7 +17127,7 @@
         <v>R-SH*Apt_KER*</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D12" s="51">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,B12,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
@@ -17164,7 +17164,7 @@
         <v>R-SH*Apt_GAS*</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D13" s="52">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,B13,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
@@ -17201,7 +17201,7 @@
         <v>R-SH*Apt_PEA*</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D14" s="51">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,B14,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
@@ -17238,7 +17238,7 @@
         <v>R-SH*Apt_SMF*</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D15" s="52">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,B15,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
@@ -17264,7 +17264,7 @@
         <v>R-SH*Apt_WOO*</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D16" s="51">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,B16,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
@@ -17290,7 +17290,7 @@
         <v>R-SH*Apt_HET*</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D17" s="52">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,B17,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
@@ -17340,7 +17340,7 @@
         <v>R-SH*Att_COA*</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D19" s="51">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H19,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
@@ -17371,7 +17371,7 @@
         <v>R-SH*Att_BDL*</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D20" s="52">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H20,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
@@ -17407,7 +17407,7 @@
         <v>R-SH*Att_ETH*</v>
       </c>
       <c r="C21" s="28" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D21" s="51">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H21,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
@@ -17443,7 +17443,7 @@
         <v>R-SH*Att_LPG*</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D22" s="52">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H22,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
@@ -17479,7 +17479,7 @@
         <v>R-S*_Att*HPN*</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D23" s="51">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H23,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
@@ -17515,7 +17515,7 @@
         <v>R-S*_Att_ELC_N1,-R-SC*</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D24" s="52">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H24,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
@@ -17551,7 +17551,7 @@
         <v>R-SH*Att_KER*</v>
       </c>
       <c r="C25" s="28" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D25" s="51">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H25,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
@@ -17583,10 +17583,10 @@
         <v>244</v>
       </c>
       <c r="B26" s="29" t="s">
-        <v>273</v>
+        <v>301</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D26" s="52">
         <f>D25</f>
@@ -17605,7 +17605,7 @@
         <v>R-SH*Att_GAS*</v>
       </c>
       <c r="C27" s="28" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D27" s="51">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H27,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
@@ -17631,7 +17631,7 @@
         <v>R-SH*Att_PEA*</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D28" s="52">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H28,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
@@ -17657,7 +17657,7 @@
         <v>R-SH*Att_SMF*</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D29" s="51">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H29,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
@@ -17683,7 +17683,7 @@
         <v>R-SH*Att_WOO*</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D30" s="52">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H30,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
@@ -17708,7 +17708,7 @@
         <v>269</v>
       </c>
       <c r="C31" s="28" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D31" s="51">
         <f>D30</f>
@@ -17727,7 +17727,7 @@
         <v>R-SH*Att_HET*</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D32" s="52">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H32,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
@@ -17765,7 +17765,7 @@
         <v>R-SH*Det_COA*</v>
       </c>
       <c r="C34" s="29" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D34" s="51">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H34,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
@@ -17791,7 +17791,7 @@
         <v>R-SH*Det_BDL*</v>
       </c>
       <c r="C35" s="29" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D35" s="52">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H35,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
@@ -17817,7 +17817,7 @@
         <v>R-SH*Det_ETH*</v>
       </c>
       <c r="C36" s="29" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D36" s="51">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H36,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
@@ -17843,7 +17843,7 @@
         <v>R-SH*Det_LPG*</v>
       </c>
       <c r="C37" s="29" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D37" s="52">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H37,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
@@ -17869,7 +17869,7 @@
         <v>R-S*_Det*HPN*</v>
       </c>
       <c r="C38" s="29" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D38" s="51">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H38,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
@@ -17895,7 +17895,7 @@
         <v>R-S*_Det_ELC_N1,-R-SC*</v>
       </c>
       <c r="C39" s="29" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D39" s="52">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H39,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
@@ -17921,7 +17921,7 @@
         <v>R-SH*Det_KER*</v>
       </c>
       <c r="C40" s="29" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D40" s="51">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H40,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
@@ -17943,10 +17943,10 @@
         <v>244</v>
       </c>
       <c r="B41" s="29" t="s">
-        <v>274</v>
+        <v>302</v>
       </c>
       <c r="C41" s="29" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D41" s="52">
         <f>D40</f>
@@ -17965,7 +17965,7 @@
         <v>R-SH*Det_GAS*</v>
       </c>
       <c r="C42" s="29" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D42" s="51">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H42,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
@@ -17991,7 +17991,7 @@
         <v>R-SH*Det_PEA*</v>
       </c>
       <c r="C43" s="29" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D43" s="52">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H43,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
@@ -18017,7 +18017,7 @@
         <v>R-SH*Det_SMF*</v>
       </c>
       <c r="C44" s="29" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D44" s="51">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H44,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
@@ -18043,7 +18043,7 @@
         <v>R-SH*Det_WOO*</v>
       </c>
       <c r="C45" s="29" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D45" s="52">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H45,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
@@ -18068,7 +18068,7 @@
         <v>270</v>
       </c>
       <c r="C46" s="29" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D46" s="51">
         <f>D45</f>
@@ -18087,7 +18087,7 @@
         <v>R-SH*Det_HET*</v>
       </c>
       <c r="C47" s="29" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D47" s="52">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H47,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
@@ -18124,7 +18124,7 @@
         <v>R-SW*Apt_COA*</v>
       </c>
       <c r="C49" s="28" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D49" s="51">
         <f>D6</f>
@@ -18150,7 +18150,7 @@
         <v>R-SW*Apt_BDL*</v>
       </c>
       <c r="C50" s="29" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D50" s="52">
         <f t="shared" ref="D50:D59" si="9">D7</f>
@@ -18176,7 +18176,7 @@
         <v>R-SW*Apt_ETH*</v>
       </c>
       <c r="C51" s="28" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D51" s="51">
         <f t="shared" si="9"/>
@@ -18202,7 +18202,7 @@
         <v>R-SW*Apt_LPG*</v>
       </c>
       <c r="C52" s="29" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D52" s="52">
         <f t="shared" si="9"/>
@@ -18228,7 +18228,7 @@
         <v>R-*_Apt*HPN*</v>
       </c>
       <c r="C53" s="28" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D53" s="51">
         <f>D10</f>
@@ -18254,7 +18254,7 @@
         <v>R-S*_Apt_ELC_N1,-R-SC*</v>
       </c>
       <c r="C54" s="29" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D54" s="52">
         <f t="shared" si="9"/>
@@ -18280,7 +18280,7 @@
         <v>R-SW*Apt_KER*</v>
       </c>
       <c r="C55" s="28" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D55" s="51">
         <f t="shared" si="9"/>
@@ -18306,7 +18306,7 @@
         <v>R-SW*Apt_GAS*</v>
       </c>
       <c r="C56" s="29" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D56" s="52">
         <f t="shared" si="9"/>
@@ -18332,7 +18332,7 @@
         <v>R-SW*Apt_PEA*</v>
       </c>
       <c r="C57" s="28" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D57" s="51">
         <f t="shared" si="9"/>
@@ -18358,7 +18358,7 @@
         <v>R-SW*Apt_SMF*</v>
       </c>
       <c r="C58" s="29" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D58" s="52">
         <f t="shared" si="9"/>
@@ -18384,7 +18384,7 @@
         <v>R-SW*Apt_WOO*</v>
       </c>
       <c r="C59" s="28" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D59" s="51">
         <f t="shared" si="9"/>
@@ -18410,7 +18410,7 @@
         <v>R-SW*Apt_HET*</v>
       </c>
       <c r="C60" s="29" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D60" s="52">
         <f>D17</f>
@@ -18448,7 +18448,7 @@
         <v>R-SW*Att_COA*</v>
       </c>
       <c r="C62" s="28" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D62" s="51">
         <f>D19</f>
@@ -18474,7 +18474,7 @@
         <v>R-SW*Att_BDL*</v>
       </c>
       <c r="C63" s="29" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D63" s="52">
         <f t="shared" ref="D63:D75" si="13">D20</f>
@@ -18500,7 +18500,7 @@
         <v>R-SW*Att_ETH*</v>
       </c>
       <c r="C64" s="28" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D64" s="51">
         <f t="shared" si="13"/>
@@ -18526,7 +18526,7 @@
         <v>R-SW*Att_LPG*</v>
       </c>
       <c r="C65" s="29" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D65" s="52">
         <f t="shared" si="13"/>
@@ -18552,7 +18552,7 @@
         <v>R-*_Att*HPN*</v>
       </c>
       <c r="C66" s="28" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D66" s="51">
         <f t="shared" si="13"/>
@@ -18578,7 +18578,7 @@
         <v>R-S*_Att_ELC_N1,-R-SC*</v>
       </c>
       <c r="C67" s="29" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D67" s="52">
         <f t="shared" si="13"/>
@@ -18604,7 +18604,7 @@
         <v>R-SW*Att_KER*</v>
       </c>
       <c r="C68" s="28" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D68" s="51">
         <f t="shared" si="13"/>
@@ -18626,10 +18626,10 @@
         <v>198</v>
       </c>
       <c r="B69" s="29" t="s">
-        <v>275</v>
+        <v>303</v>
       </c>
       <c r="C69" s="29" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D69" s="52">
         <f t="shared" si="13"/>
@@ -18648,7 +18648,7 @@
         <v>R-SW*Att_GAS*</v>
       </c>
       <c r="C70" s="28" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D70" s="51">
         <f t="shared" si="13"/>
@@ -18674,7 +18674,7 @@
         <v>R-SW*Att_PEA*</v>
       </c>
       <c r="C71" s="29" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D71" s="52">
         <f t="shared" si="13"/>
@@ -18700,7 +18700,7 @@
         <v>R-SW*Att_SMF*</v>
       </c>
       <c r="C72" s="28" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D72" s="51">
         <f t="shared" si="13"/>
@@ -18726,7 +18726,7 @@
         <v>R-SW*Att_WOO*</v>
       </c>
       <c r="C73" s="29" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D73" s="52">
         <f t="shared" si="13"/>
@@ -18751,7 +18751,7 @@
         <v>271</v>
       </c>
       <c r="C74" s="28" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D74" s="51">
         <f t="shared" si="13"/>
@@ -18770,7 +18770,7 @@
         <v>R-SW*Att_HET*</v>
       </c>
       <c r="C75" s="29" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D75" s="52">
         <f t="shared" si="13"/>
@@ -18808,7 +18808,7 @@
         <v>R-SW*Det_COA*</v>
       </c>
       <c r="C77" s="28" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D77" s="51">
         <f>D34</f>
@@ -18834,7 +18834,7 @@
         <v>R-SW*Det_BDL*</v>
       </c>
       <c r="C78" s="29" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D78" s="52">
         <f t="shared" ref="D78:D90" si="17">D35</f>
@@ -18860,7 +18860,7 @@
         <v>R-SW*Det_ETH*</v>
       </c>
       <c r="C79" s="28" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D79" s="51">
         <f t="shared" si="17"/>
@@ -18886,7 +18886,7 @@
         <v>R-SW*Det_LPG*</v>
       </c>
       <c r="C80" s="29" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D80" s="52">
         <f t="shared" si="17"/>
@@ -18912,7 +18912,7 @@
         <v>R-*_Det*HPN*</v>
       </c>
       <c r="C81" s="28" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D81" s="51">
         <f t="shared" si="17"/>
@@ -18938,7 +18938,7 @@
         <v>R-S*_Det_ELC_N1,-R-SC*</v>
       </c>
       <c r="C82" s="28" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D82" s="52">
         <f t="shared" si="17"/>
@@ -18964,7 +18964,7 @@
         <v>R-SW*Det_KER*</v>
       </c>
       <c r="C83" s="28" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D83" s="51">
         <f t="shared" si="17"/>
@@ -18986,10 +18986,10 @@
         <v>198</v>
       </c>
       <c r="B84" s="29" t="s">
-        <v>276</v>
+        <v>304</v>
       </c>
       <c r="C84" s="29" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D84" s="52">
         <f t="shared" si="17"/>
@@ -19008,7 +19008,7 @@
         <v>R-SW*Det_GAS*</v>
       </c>
       <c r="C85" s="28" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D85" s="51">
         <f t="shared" si="17"/>
@@ -19034,7 +19034,7 @@
         <v>R-SW*Det_PEA*</v>
       </c>
       <c r="C86" s="29" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D86" s="52">
         <f t="shared" si="17"/>
@@ -19060,7 +19060,7 @@
         <v>R-SW*Det_SMF*</v>
       </c>
       <c r="C87" s="28" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D87" s="51">
         <f t="shared" si="17"/>
@@ -19086,7 +19086,7 @@
         <v>R-SW*Det_WOO*</v>
       </c>
       <c r="C88" s="29" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D88" s="52">
         <f t="shared" si="17"/>
@@ -19111,7 +19111,7 @@
         <v>272</v>
       </c>
       <c r="C89" s="28" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D89" s="51">
         <f t="shared" si="17"/>
@@ -19130,7 +19130,7 @@
         <v>R-SW*Det_HET*</v>
       </c>
       <c r="C90" s="29" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D90" s="52">
         <f t="shared" si="17"/>
@@ -20253,7 +20253,7 @@
         <v>R-HC_Apt_ELC_HPN*</v>
       </c>
       <c r="C139" s="28" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="D139" s="51">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H139,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
@@ -20279,7 +20279,7 @@
         <v>R-HC_Att_ELC_HPN*</v>
       </c>
       <c r="C140" s="29" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="D140" s="52">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H140,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
@@ -20305,7 +20305,7 @@
         <v>R-HC_Det_ELC_HPN*</v>
       </c>
       <c r="C141" s="28" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="D141" s="51">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H141,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
@@ -20643,7 +20643,7 @@
         <v>R-S*_Apt_*HET*</v>
       </c>
       <c r="G16" s="28" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -20928,7 +20928,7 @@
         <v>R-S*_Att_*HET*</v>
       </c>
       <c r="G29" s="28" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -21213,7 +21213,7 @@
         <v>R-S*_Det_*HET*</v>
       </c>
       <c r="G42" s="28" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -21600,7 +21600,7 @@
         <v>R-WH_Apt_HET*</v>
       </c>
       <c r="G60" s="28" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -21908,7 +21908,7 @@
         <v>R-WH_Att_HET*</v>
       </c>
       <c r="G74" s="28" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -22216,7 +22216,7 @@
         <v>R-WH_Det_HET*</v>
       </c>
       <c r="G88" s="28" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update ETS, NOETS split
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_RSD_NewTechs_Trans.xlsx
+++ b/SubRES_TMPL/SubRES_RSD_NewTechs_Trans.xlsx
@@ -1588,7 +1588,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="7" tint="-0.499680012464523"/>
+      <color theme="7" tint="-0.499559998512268"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1603,7 +1603,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="7" tint="-0.499680012464523"/>
+      <color theme="7" tint="-0.499559998512268"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1680,7 +1680,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.0496900007128716"/>
+        <fgColor theme="0" tint="-0.0495700016617775"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1692,7 +1692,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.149700000882149"/>
+        <fgColor theme="0" tint="-0.149580001831055"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2158,7 +2158,7 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId2"/>
-        <a:srcRect l="4577" t="8892" r="7705" b="12884"/>
+        <a:srcRect l="4559" t="8874" r="7687" b="12866"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2285,7 +2285,7 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId5"/>
-        <a:srcRect l="1327" t="6523" r="3970" b="6295"/>
+        <a:srcRect l="1309" t="6504" r="3952" b="6277"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2328,7 +2328,7 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId6"/>
-        <a:srcRect l="3958" t="26158" r="3958" b="26156"/>
+        <a:srcRect l="3939" t="26139" r="3939" b="26138"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>

</xml_diff>

<commit_message>
Update ind demands and emissions
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_RSD_NewTechs_Trans.xlsx
+++ b/SubRES_TMPL/SubRES_RSD_NewTechs_Trans.xlsx
@@ -1588,7 +1588,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="7" tint="-0.499529987573624"/>
+      <color theme="7" tint="-0.499509990215302"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1603,7 +1603,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="7" tint="-0.499529987573624"/>
+      <color theme="7" tint="-0.499509990215302"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1680,7 +1680,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.0495399981737137"/>
+        <fgColor theme="0" tint="-0.0495200008153915"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1692,7 +1692,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.149550005793571"/>
+        <fgColor theme="0" tint="-0.149529993534088"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2158,7 +2158,7 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId2"/>
-        <a:srcRect l="4554" t="8869" r="7682" b="12861"/>
+        <a:srcRect l="4551" t="8866" r="7679" b="12858"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2285,7 +2285,7 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId5"/>
-        <a:srcRect l="1304" t="6500" r="3947" b="6272"/>
+        <a:srcRect l="1301" t="6497" r="3944" b="6269"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2328,7 +2328,7 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId6"/>
-        <a:srcRect l="3935" t="26135" r="3935" b="26133"/>
+        <a:srcRect l="3932" t="26132" r="3932" b="26130"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>

</xml_diff>

<commit_message>
Update demand projections and fix ambient heat bug
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_RSD_NewTechs_Trans.xlsx
+++ b/SubRES_TMPL/SubRES_RSD_NewTechs_Trans.xlsx
@@ -1044,27 +1044,27 @@
     <t>R-RSDCW_X0</t>
   </si>
   <si>
+    <t>R-LT_Det_X0</t>
+  </si>
+  <si>
+    <t>R-LT_Att_X0</t>
+  </si>
+  <si>
     <t>R-LT_Apt_X0</t>
   </si>
   <si>
-    <t>R-LT_Att_X0</t>
-  </si>
-  <si>
-    <t>R-LT_Det_X0</t>
-  </si>
-  <si>
     <t>R-RSDCD_X0</t>
   </si>
   <si>
+    <t>R-PF_Det_X0</t>
+  </si>
+  <si>
+    <t>R-PF_Att_X0</t>
+  </si>
+  <si>
     <t>R-PF_Apt_X0</t>
   </si>
   <si>
-    <t>R-PF_Att_X0</t>
-  </si>
-  <si>
-    <t>R-PF_Det_X0</t>
-  </si>
-  <si>
     <t>R-RSDDW_X0</t>
   </si>
   <si>
@@ -1308,13 +1308,13 @@
     <t>*Space Heating (dual techs)</t>
   </si>
   <si>
+    <t>R-RSDCK_LPG_X0</t>
+  </si>
+  <si>
+    <t>R-RSDCK_GAS_X0</t>
+  </si>
+  <si>
     <t>R-RSDCK_ELC_X0</t>
-  </si>
-  <si>
-    <t>R-RSDCK_GAS_X0</t>
-  </si>
-  <si>
-    <t>R-RSDCK_LPG_X0</t>
   </si>
   <si>
     <t>R-SH_Att_GAS_X0</t>
@@ -1588,7 +1588,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="7" tint="-0.499500006437302"/>
+      <color theme="7" tint="-0.499449998140335"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1603,7 +1603,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="7" tint="-0.499500006437302"/>
+      <color theme="7" tint="-0.499449998140335"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1680,7 +1680,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.0495099984109402"/>
+        <fgColor theme="0" tint="-0.0494600012898445"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1692,7 +1692,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.149519994854927"/>
+        <fgColor theme="0" tint="-0.149470001459122"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2158,7 +2158,7 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId2"/>
-        <a:srcRect l="4550" t="8865" r="7678" b="12857"/>
+        <a:srcRect l="4542" t="8857" r="7670" b="12849"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2285,7 +2285,7 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId5"/>
-        <a:srcRect l="1300" t="6495" r="3942" b="6268"/>
+        <a:srcRect l="1292" t="6488" r="3935" b="6260"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2328,7 +2328,7 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId6"/>
-        <a:srcRect l="3930" t="26130" r="3930" b="26129"/>
+        <a:srcRect l="3923" t="26123" r="3923" b="26121"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -8977,7 +8977,7 @@
         <v>78</v>
       </c>
       <c r="C2" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D2" t="s">
         <v>131</v>
@@ -9059,7 +9059,7 @@
         <v>78</v>
       </c>
       <c r="C4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D4" t="s">
         <v>131</v>
@@ -9256,7 +9256,7 @@
         <v>78</v>
       </c>
       <c r="C2" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D2" t="s">
         <v>131</v>
@@ -9338,7 +9338,7 @@
         <v>78</v>
       </c>
       <c r="C4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D4" t="s">
         <v>131</v>
@@ -9530,7 +9530,7 @@
         <v>78</v>
       </c>
       <c r="C2" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="D2" t="s">
         <v>131</v>
@@ -9612,7 +9612,7 @@
         <v>78</v>
       </c>
       <c r="C4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D4" t="s">
         <v>131</v>

</xml_diff>

<commit_message>
The model for 3rd iteration for CCAC CBWG
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_RSD_NewTechs_Trans.xlsx
+++ b/SubRES_TMPL/SubRES_RSD_NewTechs_Trans.xlsx
@@ -1588,7 +1588,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="7" tint="-0.499449998140335"/>
+      <color theme="7" tint="-0.499430000782013"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1603,7 +1603,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="7" tint="-0.499449998140335"/>
+      <color theme="7" tint="-0.499430000782013"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1680,7 +1680,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.0494600012898445"/>
+        <fgColor theme="0" tint="-0.0494400002062321"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1692,7 +1692,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.149470001459122"/>
+        <fgColor theme="0" tint="-0.1494500041008"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2158,7 +2158,7 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId2"/>
-        <a:srcRect l="4542" t="8857" r="7670" b="12849"/>
+        <a:srcRect l="4539" t="8854" r="7667" b="12846"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2285,7 +2285,7 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId5"/>
-        <a:srcRect l="1292" t="6488" r="3935" b="6260"/>
+        <a:srcRect l="1289" t="6484" r="3932" b="6257"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2328,7 +2328,7 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId6"/>
-        <a:srcRect l="3923" t="26123" r="3923" b="26121"/>
+        <a:srcRect l="3919" t="26119" r="3919" b="26118"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -11829,7 +11829,7 @@
       <c r="C6" s="33"/>
       <c r="D6" s="55">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,B6,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>0.40654789002485697</v>
+        <v>0.12</v>
       </c>
       <c r="F6" s="33" t="s">
         <v>109</v>
@@ -11864,7 +11864,7 @@
       <c r="C7" s="34"/>
       <c r="D7" s="56">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,B7,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>0.0096640000122913006</v>
+        <v>0.12</v>
       </c>
       <c r="F7" s="34" t="s">
         <v>109</v>
@@ -11899,7 +11899,7 @@
       <c r="C8" s="33"/>
       <c r="D8" s="55">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,B8,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>2.0797704474084602E-05</v>
+        <v>0.12</v>
       </c>
       <c r="F8" s="33" t="s">
         <v>109</v>
@@ -11934,7 +11934,7 @@
       <c r="C9" s="34"/>
       <c r="D9" s="56">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,B9,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>0.047559865677763699</v>
+        <v>0.12</v>
       </c>
       <c r="F9" s="34" t="s">
         <v>109</v>
@@ -12144,7 +12144,7 @@
       <c r="C15" s="34"/>
       <c r="D15" s="56">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,B15,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>0.14274595375996399</v>
+        <v>0.12</v>
       </c>
       <c r="F15" s="34" t="s">
         <v>109</v>
@@ -12168,7 +12168,7 @@
       <c r="C16" s="33"/>
       <c r="D16" s="55">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,B16,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>0.036221240391349503</v>
+        <v>0.12</v>
       </c>
       <c r="F16" s="33" t="s">
         <v>109</v>
@@ -12192,7 +12192,7 @@
       <c r="C17" s="34"/>
       <c r="D17" s="56">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,B17,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>0.0024002855672672599</v>
+        <v>0.12</v>
       </c>
       <c r="F17" s="34" t="s">
         <v>109</v>
@@ -12269,7 +12269,7 @@
       <c r="C20" s="34"/>
       <c r="D20" s="56">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H20,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>0.0253147717385124</v>
+        <v>0.12</v>
       </c>
       <c r="F20" s="34" t="s">
         <v>105</v>
@@ -12303,7 +12303,7 @@
       <c r="C21" s="33"/>
       <c r="D21" s="55">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H21,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>0</v>
+        <v>0.12</v>
       </c>
       <c r="F21" s="33" t="s">
         <v>105</v>
@@ -12564,7 +12564,7 @@
       <c r="C30" s="34"/>
       <c r="D30" s="56">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H30,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>0.11656908094434699</v>
+        <v>0.12</v>
       </c>
       <c r="F30" s="34" t="s">
         <v>105</v>
@@ -12587,7 +12587,7 @@
       <c r="C31" s="33"/>
       <c r="D31" s="55">
         <f>D30</f>
-        <v>0.11656908094434699</v>
+        <v>0.12</v>
       </c>
       <c r="F31" s="33"/>
       <c r="G31" s="33"/>
@@ -12604,7 +12604,7 @@
       <c r="C32" s="34"/>
       <c r="D32" s="56">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H32,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>0.023481233276961201</v>
+        <v>0.12</v>
       </c>
       <c r="F32" s="34" t="s">
         <v>105</v>
@@ -12664,7 +12664,7 @@
       <c r="C35" s="34"/>
       <c r="D35" s="56">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H35,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>0</v>
+        <v>0.0697946718860816</v>
       </c>
       <c r="F35" s="34" t="s">
         <v>114</v>
@@ -12688,7 +12688,7 @@
       <c r="C36" s="33"/>
       <c r="D36" s="55">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H36,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>0</v>
+        <v>0.0697946718860816</v>
       </c>
       <c r="F36" s="33" t="s">
         <v>114</v>
@@ -12936,7 +12936,7 @@
       <c r="C47" s="34"/>
       <c r="D47" s="56">
         <f>AVERAGEIFS('BY-RSD-SH_AF'!$L$2:$L$100,'BY-RSD-SH_AF'!$C$2:$C$100,H47,'BY-RSD-SH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>0.203493994761373</v>
+        <v>0.12</v>
       </c>
       <c r="F47" s="34" t="s">
         <v>114</v>
@@ -12973,7 +12973,7 @@
       </c>
       <c r="D49" s="55">
         <f>D6</f>
-        <v>0.40654789002485697</v>
+        <v>0.12</v>
       </c>
       <c r="F49" s="33" t="s">
         <v>109</v>
@@ -12999,7 +12999,7 @@
       </c>
       <c r="D50" s="56">
         <f t="shared" si="9" ref="D50:D59">D7</f>
-        <v>0.0096640000122913006</v>
+        <v>0.12</v>
       </c>
       <c r="F50" s="34" t="s">
         <v>109</v>
@@ -13025,7 +13025,7 @@
       </c>
       <c r="D51" s="55">
         <f t="shared" si="9"/>
-        <v>2.0797704474084602E-05</v>
+        <v>0.12</v>
       </c>
       <c r="F51" s="33" t="s">
         <v>109</v>
@@ -13051,7 +13051,7 @@
       </c>
       <c r="D52" s="56">
         <f t="shared" si="9"/>
-        <v>0.047559865677763699</v>
+        <v>0.12</v>
       </c>
       <c r="F52" s="34" t="s">
         <v>109</v>
@@ -13207,7 +13207,7 @@
       </c>
       <c r="D58" s="56">
         <f t="shared" si="9"/>
-        <v>0.14274595375996399</v>
+        <v>0.12</v>
       </c>
       <c r="F58" s="34" t="s">
         <v>109</v>
@@ -13233,7 +13233,7 @@
       </c>
       <c r="D59" s="55">
         <f t="shared" si="9"/>
-        <v>0.036221240391349503</v>
+        <v>0.12</v>
       </c>
       <c r="F59" s="33" t="s">
         <v>109</v>
@@ -13259,7 +13259,7 @@
       </c>
       <c r="D60" s="56">
         <f>D17</f>
-        <v>0.0024002855672672599</v>
+        <v>0.12</v>
       </c>
       <c r="F60" s="34" t="s">
         <v>109</v>
@@ -13323,7 +13323,7 @@
       </c>
       <c r="D63" s="56">
         <f t="shared" si="13" ref="D63:D75">D20</f>
-        <v>0.0253147717385124</v>
+        <v>0.12</v>
       </c>
       <c r="F63" s="34" t="s">
         <v>105</v>
@@ -13349,7 +13349,7 @@
       </c>
       <c r="D64" s="55">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>0.12</v>
       </c>
       <c r="F64" s="33" t="s">
         <v>105</v>
@@ -13575,7 +13575,7 @@
       </c>
       <c r="D73" s="56">
         <f t="shared" si="13"/>
-        <v>0.11656908094434699</v>
+        <v>0.12</v>
       </c>
       <c r="F73" s="34" t="s">
         <v>105</v>
@@ -13600,7 +13600,7 @@
       </c>
       <c r="D74" s="55">
         <f t="shared" si="13"/>
-        <v>0.11656908094434699</v>
+        <v>0.12</v>
       </c>
       <c r="F74" s="33"/>
       <c r="G74" s="33"/>
@@ -13619,7 +13619,7 @@
       </c>
       <c r="D75" s="56">
         <f t="shared" si="13"/>
-        <v>0.023481233276961201</v>
+        <v>0.12</v>
       </c>
       <c r="F75" s="34" t="s">
         <v>105</v>
@@ -13683,7 +13683,7 @@
       </c>
       <c r="D78" s="56">
         <f t="shared" si="17" ref="D78:D90">D35</f>
-        <v>0</v>
+        <v>0.0697946718860816</v>
       </c>
       <c r="F78" s="34" t="s">
         <v>114</v>
@@ -13709,7 +13709,7 @@
       </c>
       <c r="D79" s="55">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>0.0697946718860816</v>
       </c>
       <c r="F79" s="33" t="s">
         <v>114</v>
@@ -13979,7 +13979,7 @@
       </c>
       <c r="D90" s="56">
         <f t="shared" si="17"/>
-        <v>0.203493994761373</v>
+        <v>0.12</v>
       </c>
       <c r="F90" s="34" t="s">
         <v>114</v>
@@ -14014,7 +14014,7 @@
       <c r="C92" s="33"/>
       <c r="D92" s="55">
         <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H92,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>0.42342871317737102</v>
+        <v>0.12</v>
       </c>
       <c r="F92" s="33" t="s">
         <v>109</v>
@@ -14038,7 +14038,7 @@
       <c r="C93" s="34"/>
       <c r="D93" s="56">
         <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H93,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>0.075051369863013695</v>
+        <v>0.12</v>
       </c>
       <c r="F93" s="34" t="s">
         <v>109</v>
@@ -14062,7 +14062,7 @@
       <c r="C94" s="33"/>
       <c r="D94" s="55">
         <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H94,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>0.090422374429223698</v>
+        <v>0.12</v>
       </c>
       <c r="F94" s="33" t="s">
         <v>109</v>
@@ -14086,7 +14086,7 @@
       <c r="C95" s="34"/>
       <c r="D95" s="56">
         <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H95,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>0.12792665468435199</v>
+        <v>0.12</v>
       </c>
       <c r="F95" s="34" t="s">
         <v>109</v>
@@ -14134,7 +14134,7 @@
       <c r="C97" s="34"/>
       <c r="D97" s="56">
         <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H97,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>0.11252568167857099</v>
+        <v>0.12</v>
       </c>
       <c r="F97" s="34" t="s">
         <v>109</v>
@@ -14182,7 +14182,7 @@
       <c r="C99" s="34"/>
       <c r="D99" s="56">
         <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H99,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>0.090627195293291204</v>
+        <v>0.12</v>
       </c>
       <c r="F99" s="34" t="s">
         <v>109</v>
@@ -14206,7 +14206,7 @@
       <c r="C100" s="33"/>
       <c r="D100" s="55">
         <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H100,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>0.0867381932124731</v>
+        <v>0.12</v>
       </c>
       <c r="F100" s="33" t="s">
         <v>109</v>
@@ -14230,7 +14230,7 @@
       <c r="C101" s="34"/>
       <c r="D101" s="56">
         <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H101,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>0.099394310243560199</v>
+        <v>0.12</v>
       </c>
       <c r="F101" s="34" t="s">
         <v>109</v>
@@ -14254,7 +14254,7 @@
       <c r="C102" s="33"/>
       <c r="D102" s="55">
         <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H102,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>0.0032373195740855901</v>
+        <v>0.12</v>
       </c>
       <c r="F102" s="33" t="s">
         <v>109</v>
@@ -14338,7 +14338,7 @@
       <c r="C106" s="34"/>
       <c r="D106" s="56">
         <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H106,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>0.088919330289193299</v>
+        <v>0.12</v>
       </c>
       <c r="F106" s="34" t="s">
         <v>105</v>
@@ -14362,7 +14362,7 @@
       <c r="C107" s="33"/>
       <c r="D107" s="55">
         <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H107,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>0.067212328767123297</v>
+        <v>0.12</v>
       </c>
       <c r="F107" s="33" t="s">
         <v>105</v>
@@ -14386,7 +14386,7 @@
       <c r="C108" s="34"/>
       <c r="D108" s="56">
         <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H108,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>0.0973639647341112</v>
+        <v>0.12</v>
       </c>
       <c r="F108" s="34" t="s">
         <v>105</v>
@@ -14482,7 +14482,7 @@
       <c r="C112" s="34"/>
       <c r="D112" s="56">
         <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H112,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>0.068944308925102102</v>
+        <v>0.12</v>
       </c>
       <c r="F112" s="34" t="s">
         <v>105</v>
@@ -14530,7 +14530,7 @@
       <c r="C114" s="34"/>
       <c r="D114" s="56">
         <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H114,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>0.066620869969995597</v>
+        <v>0.12</v>
       </c>
       <c r="F114" s="34" t="s">
         <v>105</v>
@@ -14554,7 +14554,7 @@
       <c r="C115" s="33"/>
       <c r="D115" s="55">
         <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H115,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>0.0048794584261943399</v>
+        <v>0.12</v>
       </c>
       <c r="F115" s="33" t="s">
         <v>105</v>
@@ -14614,7 +14614,7 @@
       <c r="C118" s="33"/>
       <c r="D118" s="55">
         <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H118,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>0.070651721487066402</v>
+        <v>0.12</v>
       </c>
       <c r="F118" s="33" t="s">
         <v>114</v>
@@ -14638,7 +14638,7 @@
       <c r="C119" s="34"/>
       <c r="D119" s="56">
         <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H119,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>0.042328767123287703</v>
+        <v>0.12</v>
       </c>
       <c r="F119" s="34" t="s">
         <v>114</v>
@@ -14662,7 +14662,7 @@
       <c r="C120" s="33"/>
       <c r="D120" s="55">
         <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H120,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>0.047947345890410997</v>
+        <v>0.12</v>
       </c>
       <c r="F120" s="33" t="s">
         <v>114</v>
@@ -14686,7 +14686,7 @@
       <c r="C121" s="34"/>
       <c r="D121" s="56">
         <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H121,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>0.067402586104361395</v>
+        <v>0.12</v>
       </c>
       <c r="F121" s="34" t="s">
         <v>114</v>
@@ -14710,7 +14710,7 @@
       <c r="C122" s="33"/>
       <c r="D122" s="55">
         <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H122,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>0.044735473424353099</v>
+        <v>0.12</v>
       </c>
       <c r="F122" s="33" t="s">
         <v>114</v>
@@ -14782,7 +14782,7 @@
       <c r="C125" s="34"/>
       <c r="D125" s="56">
         <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H125,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>0.023589745043839899</v>
+        <v>0.12</v>
       </c>
       <c r="F125" s="34" t="s">
         <v>114</v>
@@ -14830,7 +14830,7 @@
       <c r="C127" s="34"/>
       <c r="D127" s="56">
         <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H127,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>0.056573502855343599</v>
+        <v>0.12</v>
       </c>
       <c r="F127" s="34" t="s">
         <v>114</v>
@@ -14854,7 +14854,7 @@
       <c r="C128" s="33"/>
       <c r="D128" s="55">
         <f>AVERAGEIFS('BY-RSD-WH_AF'!$L$2:$L$100,'BY-RSD-WH_AF'!$C$2:$C$100,H128,'BY-RSD-WH_AF'!$A$2:$A$100,"BASE")</f>
-        <v>0.0051032329364559198</v>
+        <v>0.12</v>
       </c>
       <c r="F128" s="33" t="s">
         <v>114</v>
@@ -17162,10 +17162,10 @@
         <v>131</v>
       </c>
       <c r="L2">
-        <v>0.075051369863013695</v>
+        <v>0.12</v>
       </c>
       <c r="M2">
-        <v>0.075051369863013695</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="12.75">
@@ -17203,10 +17203,10 @@
         <v>131</v>
       </c>
       <c r="L3">
-        <v>0.42342871317737102</v>
+        <v>0.12</v>
       </c>
       <c r="M3">
-        <v>0.42342871317737102</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="12.75">
@@ -17326,10 +17326,10 @@
         <v>131</v>
       </c>
       <c r="L6">
-        <v>0.090422374429223698</v>
+        <v>0.12</v>
       </c>
       <c r="M6">
-        <v>0.090422374429223698</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="12.75">
@@ -17408,10 +17408,10 @@
         <v>131</v>
       </c>
       <c r="L8">
-        <v>0.0032373195740855901</v>
+        <v>0.12</v>
       </c>
       <c r="M8">
-        <v>0.0032373195740855901</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="12.75">
@@ -17449,10 +17449,10 @@
         <v>131</v>
       </c>
       <c r="L9">
-        <v>0.11252568167857099</v>
+        <v>0.12</v>
       </c>
       <c r="M9">
-        <v>0.11252568167857099</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="12.75">
@@ -17490,10 +17490,10 @@
         <v>131</v>
       </c>
       <c r="L10">
-        <v>0.12792665468435199</v>
+        <v>0.12</v>
       </c>
       <c r="M10">
-        <v>0.12792665468435199</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="12.75">
@@ -17531,10 +17531,10 @@
         <v>131</v>
       </c>
       <c r="L11">
-        <v>0.090627195293291204</v>
+        <v>0.12</v>
       </c>
       <c r="M11">
-        <v>0.090627195293291204</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="12.75">
@@ -17572,10 +17572,10 @@
         <v>131</v>
       </c>
       <c r="L12">
-        <v>0.0867381932124731</v>
+        <v>0.12</v>
       </c>
       <c r="M12">
-        <v>0.0867381932124731</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="12.75">
@@ -17654,10 +17654,10 @@
         <v>131</v>
       </c>
       <c r="L14">
-        <v>0.099394310243560199</v>
+        <v>0.12</v>
       </c>
       <c r="M14">
-        <v>0.099394310243560199</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="12.75">
@@ -17695,10 +17695,10 @@
         <v>131</v>
       </c>
       <c r="L15">
-        <v>0.088919330289193299</v>
+        <v>0.12</v>
       </c>
       <c r="M15">
-        <v>0.088919330289193299</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="12.75">
@@ -17859,10 +17859,10 @@
         <v>131</v>
       </c>
       <c r="L19">
-        <v>0.067212328767123297</v>
+        <v>0.12</v>
       </c>
       <c r="M19">
-        <v>0.067212328767123297</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="12.75">
@@ -17941,10 +17941,10 @@
         <v>131</v>
       </c>
       <c r="L21">
-        <v>0.0048794584261943399</v>
+        <v>0.12</v>
       </c>
       <c r="M21">
-        <v>0.0048794584261943399</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="12.75">
@@ -18023,10 +18023,10 @@
         <v>131</v>
       </c>
       <c r="L23">
-        <v>0.0973639647341112</v>
+        <v>0.12</v>
       </c>
       <c r="M23">
-        <v>0.0973639647341112</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="12.75">
@@ -18064,10 +18064,10 @@
         <v>131</v>
       </c>
       <c r="L24">
-        <v>0.068944308925102102</v>
+        <v>0.12</v>
       </c>
       <c r="M24">
-        <v>0.068944308925102102</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="12.75">
@@ -18187,10 +18187,10 @@
         <v>131</v>
       </c>
       <c r="L27">
-        <v>0.066620869969995597</v>
+        <v>0.12</v>
       </c>
       <c r="M27">
-        <v>0.066620869969995597</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="12.75">
@@ -18228,10 +18228,10 @@
         <v>131</v>
       </c>
       <c r="L28">
-        <v>0.042328767123287703</v>
+        <v>0.12</v>
       </c>
       <c r="M28">
-        <v>0.042328767123287703</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="12.75">
@@ -18269,10 +18269,10 @@
         <v>131</v>
       </c>
       <c r="L29">
-        <v>0.070651721487066402</v>
+        <v>0.12</v>
       </c>
       <c r="M29">
-        <v>0.070651721487066402</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="12.75">
@@ -18310,10 +18310,10 @@
         <v>131</v>
       </c>
       <c r="L30">
-        <v>0.044735473424353099</v>
+        <v>0.12</v>
       </c>
       <c r="M30">
-        <v>0.044735473424353099</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="12.75">
@@ -18351,10 +18351,10 @@
         <v>131</v>
       </c>
       <c r="L31">
-        <v>0.458133885220118</v>
+        <v>0.12</v>
       </c>
       <c r="M31">
-        <v>0.458133885220118</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="12.75">
@@ -18392,10 +18392,10 @@
         <v>131</v>
       </c>
       <c r="L32">
-        <v>0.047947345890410997</v>
+        <v>0.12</v>
       </c>
       <c r="M32">
-        <v>0.047947345890410997</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="12.75">
@@ -18474,10 +18474,10 @@
         <v>131</v>
       </c>
       <c r="L34">
-        <v>0.0051032329364559198</v>
+        <v>0.12</v>
       </c>
       <c r="M34">
-        <v>0.0051032329364559198</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="12.75">
@@ -18556,10 +18556,10 @@
         <v>131</v>
       </c>
       <c r="L36">
-        <v>0.067402586104361395</v>
+        <v>0.12</v>
       </c>
       <c r="M36">
-        <v>0.067402586104361395</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="12.75">
@@ -18597,10 +18597,10 @@
         <v>131</v>
       </c>
       <c r="L37">
-        <v>0.023589745043839899</v>
+        <v>0.12</v>
       </c>
       <c r="M37">
-        <v>0.023589745043839899</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="12.75">
@@ -18720,10 +18720,10 @@
         <v>131</v>
       </c>
       <c r="L40">
-        <v>0.056573502855343599</v>
+        <v>0.12</v>
       </c>
       <c r="M40">
-        <v>0.056573502855343599</v>
+        <v>0.12</v>
       </c>
     </row>
   </sheetData>
@@ -18819,10 +18819,10 @@
         <v>131</v>
       </c>
       <c r="L2">
-        <v>0.0096640000122913006</v>
+        <v>0.12</v>
       </c>
       <c r="M2">
-        <v>0.0096640000122913006</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="12.75">
@@ -18860,10 +18860,10 @@
         <v>131</v>
       </c>
       <c r="L3">
-        <v>0.40654789002485697</v>
+        <v>0.12</v>
       </c>
       <c r="M3">
-        <v>0.40654789002485697</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="12.75">
@@ -18983,10 +18983,10 @@
         <v>131</v>
       </c>
       <c r="L6">
-        <v>2.0797704474084602E-05</v>
+        <v>0.12</v>
       </c>
       <c r="M6">
-        <v>2.0797704474084602E-05</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="12.75">
@@ -19065,10 +19065,10 @@
         <v>131</v>
       </c>
       <c r="L8">
-        <v>0.0024002855672672599</v>
+        <v>0.12</v>
       </c>
       <c r="M8">
-        <v>0.0024002855672672599</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="12.75">
@@ -19147,10 +19147,10 @@
         <v>131</v>
       </c>
       <c r="L10">
-        <v>0.047559865677763699</v>
+        <v>0.12</v>
       </c>
       <c r="M10">
-        <v>0.047559865677763699</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="12.75">
@@ -19229,10 +19229,10 @@
         <v>131</v>
       </c>
       <c r="L12">
-        <v>0.14274595375996399</v>
+        <v>0.12</v>
       </c>
       <c r="M12">
-        <v>0.14274595375996399</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="12.75">
@@ -19270,10 +19270,10 @@
         <v>131</v>
       </c>
       <c r="L13">
-        <v>0.036221240391349503</v>
+        <v>0.12</v>
       </c>
       <c r="M13">
-        <v>0.036221240391349503</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="12.75">
@@ -19311,10 +19311,10 @@
         <v>131</v>
       </c>
       <c r="L14">
-        <v>0.0253147717385124</v>
+        <v>0.12</v>
       </c>
       <c r="M14">
-        <v>0.0253147717385124</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="12.75">
@@ -19475,10 +19475,10 @@
         <v>131</v>
       </c>
       <c r="L18">
-        <v>0</v>
+        <v>0.12</v>
       </c>
       <c r="M18">
-        <v>0</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="12.75">
@@ -19557,10 +19557,10 @@
         <v>131</v>
       </c>
       <c r="L20">
-        <v>0.023481233276961201</v>
+        <v>0.12</v>
       </c>
       <c r="M20">
-        <v>0.023481233276961201</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="12.75">
@@ -19762,10 +19762,10 @@
         <v>131</v>
       </c>
       <c r="L25">
-        <v>0.11656908094434699</v>
+        <v>0.12</v>
       </c>
       <c r="M25">
-        <v>0.11656908094434699</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="12.75">
@@ -19803,10 +19803,10 @@
         <v>131</v>
       </c>
       <c r="L26">
-        <v>0</v>
+        <v>0.0697946718860816</v>
       </c>
       <c r="M26">
-        <v>0</v>
+        <v>0.0697946718860816</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="12.75">
@@ -19967,10 +19967,10 @@
         <v>131</v>
       </c>
       <c r="L30">
-        <v>0</v>
+        <v>0.0697946718860816</v>
       </c>
       <c r="M30">
-        <v>0</v>
+        <v>0.0697946718860816</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="12.75">
@@ -20049,10 +20049,10 @@
         <v>131</v>
       </c>
       <c r="L32">
-        <v>0.203493994761373</v>
+        <v>0.12</v>
       </c>
       <c r="M32">
-        <v>0.203493994761373</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="12.75">

</xml_diff>

<commit_message>
Update demand projections for industry
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_RSD_NewTechs_Trans.xlsx
+++ b/SubRES_TMPL/SubRES_RSD_NewTechs_Trans.xlsx
@@ -1044,27 +1044,27 @@
     <t>R-RSDCW_X0</t>
   </si>
   <si>
+    <t>R-LT_Apt_X0</t>
+  </si>
+  <si>
+    <t>R-LT_Att_X0</t>
+  </si>
+  <si>
     <t>R-LT_Det_X0</t>
   </si>
   <si>
-    <t>R-LT_Att_X0</t>
-  </si>
-  <si>
-    <t>R-LT_Apt_X0</t>
-  </si>
-  <si>
     <t>R-RSDCD_X0</t>
   </si>
   <si>
+    <t>R-PF_Apt_X0</t>
+  </si>
+  <si>
+    <t>R-PF_Att_X0</t>
+  </si>
+  <si>
     <t>R-PF_Det_X0</t>
   </si>
   <si>
-    <t>R-PF_Att_X0</t>
-  </si>
-  <si>
-    <t>R-PF_Apt_X0</t>
-  </si>
-  <si>
     <t>R-RSDDW_X0</t>
   </si>
   <si>
@@ -1308,13 +1308,13 @@
     <t>*Space Heating (dual techs)</t>
   </si>
   <si>
+    <t>R-RSDCK_ELC_X0</t>
+  </si>
+  <si>
+    <t>R-RSDCK_GAS_X0</t>
+  </si>
+  <si>
     <t>R-RSDCK_LPG_X0</t>
-  </si>
-  <si>
-    <t>R-RSDCK_GAS_X0</t>
-  </si>
-  <si>
-    <t>R-RSDCK_ELC_X0</t>
   </si>
   <si>
     <t>R-SH_Att_GAS_X0</t>
@@ -1588,7 +1588,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="7" tint="-0.499430000782013"/>
+      <color theme="7" tint="-0.499419987201691"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1603,7 +1603,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="7" tint="-0.499430000782013"/>
+      <color theme="7" tint="-0.499419987201691"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1680,7 +1680,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.0494400002062321"/>
+        <fgColor theme="0" tint="-0.049430001527071"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1692,7 +1692,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.1494500041008"/>
+        <fgColor theme="0" tint="-0.149440005421638"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2158,7 +2158,7 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId2"/>
-        <a:srcRect l="4539" t="8854" r="7667" b="12846"/>
+        <a:srcRect l="4537" t="8853" r="7666" b="12844"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2285,7 +2285,7 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId5"/>
-        <a:srcRect l="1289" t="6484" r="3932" b="6257"/>
+        <a:srcRect l="1287" t="6483" r="3930" b="6256"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2328,7 +2328,7 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId6"/>
-        <a:srcRect l="3919" t="26119" r="3919" b="26118"/>
+        <a:srcRect l="3918" t="26118" r="3918" b="26116"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -8977,7 +8977,7 @@
         <v>78</v>
       </c>
       <c r="C2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D2" t="s">
         <v>131</v>
@@ -9059,7 +9059,7 @@
         <v>78</v>
       </c>
       <c r="C4" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D4" t="s">
         <v>131</v>
@@ -9256,7 +9256,7 @@
         <v>78</v>
       </c>
       <c r="C2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D2" t="s">
         <v>131</v>
@@ -9338,7 +9338,7 @@
         <v>78</v>
       </c>
       <c r="C4" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D4" t="s">
         <v>131</v>
@@ -9530,7 +9530,7 @@
         <v>78</v>
       </c>
       <c r="C2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D2" t="s">
         <v>131</v>
@@ -9612,7 +9612,7 @@
         <v>78</v>
       </c>
       <c r="C4" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="D4" t="s">
         <v>131</v>

</xml_diff>